<commit_message>
increase font size for inputfield
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malik/Desktop/Extras/acc/Expences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9E2AEA-0CC7-1542-9603-E059277EA72C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96379153-7308-5E42-A586-94636DA16108}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -236,7 +236,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d&quot;-&quot;mmm"/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="37">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -471,6 +471,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1066,6 +1073,9 @@
     <xf numFmtId="0" fontId="33" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="19" borderId="9" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1093,10 +1103,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="18" borderId="8" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="19" borderId="9" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="18" borderId="8" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1419,14 +1426,14 @@
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="138" t="s">
+      <c r="J1" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="139"/>
-      <c r="L1" s="140" t="s">
+      <c r="K1" s="140"/>
+      <c r="L1" s="141" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="139"/>
+      <c r="M1" s="140"/>
       <c r="N1" s="6"/>
       <c r="O1" s="7" t="s">
         <v>9</v>
@@ -1446,15 +1453,15 @@
       </c>
       <c r="U1" s="8"/>
       <c r="V1" s="9"/>
-      <c r="W1" s="141" t="s">
+      <c r="W1" s="142" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="142"/>
-      <c r="Y1" s="142"/>
-      <c r="Z1" s="142"/>
-      <c r="AA1" s="142"/>
-      <c r="AB1" s="142"/>
-      <c r="AC1" s="139"/>
+      <c r="X1" s="143"/>
+      <c r="Y1" s="143"/>
+      <c r="Z1" s="143"/>
+      <c r="AA1" s="143"/>
+      <c r="AB1" s="143"/>
+      <c r="AC1" s="140"/>
       <c r="AD1" s="2"/>
       <c r="AE1" s="2"/>
       <c r="AF1" s="2"/>
@@ -1634,7 +1641,7 @@
         <f>SUM(Q2/B10)</f>
         <v>27.339999999999996</v>
       </c>
-      <c r="R4" s="143">
+      <c r="R4" s="144">
         <v>800</v>
       </c>
       <c r="S4" s="35"/>
@@ -1718,7 +1725,7 @@
         <f>SUM(Q2/B10)</f>
         <v>27.339999999999996</v>
       </c>
-      <c r="R5" s="144"/>
+      <c r="R5" s="145"/>
       <c r="S5" s="35"/>
       <c r="T5" s="49">
         <f t="shared" si="2"/>
@@ -1800,7 +1807,7 @@
         <f>SUM(Q2/B10)</f>
         <v>27.339999999999996</v>
       </c>
-      <c r="R6" s="143">
+      <c r="R6" s="144">
         <v>700</v>
       </c>
       <c r="S6" s="35"/>
@@ -1884,7 +1891,7 @@
         <f>SUM(Q2/B10)</f>
         <v>27.339999999999996</v>
       </c>
-      <c r="R7" s="144"/>
+      <c r="R7" s="145"/>
       <c r="S7" s="35"/>
       <c r="T7" s="49">
         <f t="shared" si="2"/>
@@ -2242,7 +2249,7 @@
       <c r="V17" s="27"/>
     </row>
     <row r="18" spans="1:22" ht="13">
-      <c r="A18" s="135" t="s">
+      <c r="A18" s="136" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="69" t="b">
@@ -2269,7 +2276,7 @@
       <c r="V18" s="27"/>
     </row>
     <row r="19" spans="1:22" ht="13">
-      <c r="A19" s="137"/>
+      <c r="A19" s="138"/>
       <c r="B19" s="70" t="b">
         <v>0</v>
       </c>
@@ -2294,7 +2301,7 @@
       <c r="V19" s="27"/>
     </row>
     <row r="20" spans="1:22" ht="14">
-      <c r="A20" s="135" t="s">
+      <c r="A20" s="136" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="71" t="s">
@@ -2321,7 +2328,7 @@
       <c r="V20" s="27"/>
     </row>
     <row r="21" spans="1:22" ht="13">
-      <c r="A21" s="136"/>
+      <c r="A21" s="137"/>
       <c r="B21" s="71" t="s">
         <v>2</v>
       </c>
@@ -2346,7 +2353,7 @@
       <c r="V21" s="27"/>
     </row>
     <row r="22" spans="1:22" ht="13">
-      <c r="A22" s="137"/>
+      <c r="A22" s="138"/>
       <c r="B22" s="71" t="s">
         <v>40</v>
       </c>
@@ -2371,7 +2378,7 @@
       <c r="V22" s="27"/>
     </row>
     <row r="23" spans="1:22" ht="13">
-      <c r="A23" s="135" t="s">
+      <c r="A23" s="136" t="s">
         <v>41</v>
       </c>
       <c r="B23" s="73">
@@ -2398,7 +2405,7 @@
       <c r="V23" s="27"/>
     </row>
     <row r="24" spans="1:22" ht="13">
-      <c r="A24" s="136"/>
+      <c r="A24" s="137"/>
       <c r="B24" s="73">
         <v>7</v>
       </c>
@@ -2423,7 +2430,7 @@
       <c r="V24" s="27"/>
     </row>
     <row r="25" spans="1:22" ht="13">
-      <c r="A25" s="137"/>
+      <c r="A25" s="138"/>
       <c r="B25" s="73">
         <v>5</v>
       </c>
@@ -2448,7 +2455,7 @@
       <c r="V25" s="27"/>
     </row>
     <row r="26" spans="1:22" ht="13">
-      <c r="A26" s="135" t="s">
+      <c r="A26" s="136" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="74">
@@ -2475,7 +2482,7 @@
       <c r="V26" s="27"/>
     </row>
     <row r="27" spans="1:22" ht="13">
-      <c r="A27" s="137"/>
+      <c r="A27" s="138"/>
       <c r="B27" s="74">
         <v>165</v>
       </c>
@@ -25083,7 +25090,7 @@
       <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -25107,14 +25114,14 @@
       <c r="D1" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="145"/>
+      <c r="E1" s="146"/>
       <c r="F1" s="81"/>
       <c r="G1" s="82"/>
       <c r="H1" s="83"/>
       <c r="I1" s="83"/>
       <c r="J1" s="83"/>
       <c r="K1" s="84"/>
-      <c r="L1" s="146"/>
+      <c r="L1" s="147"/>
       <c r="M1" s="32"/>
       <c r="N1" s="86" t="s">
         <v>46</v>
@@ -25150,17 +25157,17 @@
       <c r="C2" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="150">
+      <c r="D2" s="151">
         <v>30</v>
       </c>
-      <c r="E2" s="144"/>
+      <c r="E2" s="145"/>
       <c r="F2" s="91"/>
       <c r="G2" s="89"/>
       <c r="H2" s="89"/>
       <c r="I2" s="89"/>
       <c r="J2" s="89"/>
       <c r="K2" s="89"/>
-      <c r="L2" s="144"/>
+      <c r="L2" s="145"/>
       <c r="M2" s="81"/>
       <c r="N2" s="92"/>
       <c r="O2" s="93">
@@ -25203,13 +25210,13 @@
       <c r="G3" s="134" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="150">
+      <c r="H3" s="151">
         <v>0</v>
       </c>
-      <c r="I3" s="150">
+      <c r="I3" s="151">
         <v>0</v>
       </c>
-      <c r="J3" s="150">
+      <c r="J3" s="151">
         <v>136.69999999999999</v>
       </c>
       <c r="K3" s="100">
@@ -25220,7 +25227,7 @@
         <v>136.69999999999999</v>
       </c>
       <c r="M3" s="102"/>
-      <c r="N3" s="150" t="s">
+      <c r="N3" s="151" t="s">
         <v>67</v>
       </c>
       <c r="O3" s="103" t="str">
@@ -25299,10 +25306,10 @@
         <f t="shared" si="0"/>
         <v>165</v>
       </c>
-      <c r="D5" s="151" t="s">
+      <c r="D5" s="135" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="147"/>
+      <c r="E5" s="148"/>
       <c r="F5" s="81"/>
       <c r="G5" s="112">
         <f>Manager!T4</f>
@@ -25324,7 +25331,7 @@
         <f>SUM(K3/5)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="148"/>
+      <c r="L5" s="149"/>
       <c r="M5" s="32"/>
       <c r="N5" s="117">
         <v>7</v>
@@ -25365,10 +25372,10 @@
         <f t="shared" si="1"/>
         <v>165</v>
       </c>
-      <c r="D6" s="151" t="s">
+      <c r="D6" s="135" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="144"/>
+      <c r="E6" s="145"/>
       <c r="F6" s="81"/>
       <c r="G6" s="112">
         <f>Manager!T5</f>
@@ -25390,7 +25397,7 @@
         <f>SUM(K3/5)</f>
         <v>0</v>
       </c>
-      <c r="L6" s="144"/>
+      <c r="L6" s="145"/>
       <c r="M6" s="32"/>
       <c r="N6" s="117">
         <v>7</v>
@@ -25431,10 +25438,10 @@
         <f t="shared" si="2"/>
         <v>165</v>
       </c>
-      <c r="D7" s="151" t="s">
+      <c r="D7" s="135" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="144"/>
+      <c r="E7" s="145"/>
       <c r="F7" s="81"/>
       <c r="G7" s="112">
         <f>Manager!T6</f>
@@ -25456,7 +25463,7 @@
         <f>SUM(K3/5)</f>
         <v>0</v>
       </c>
-      <c r="L7" s="144"/>
+      <c r="L7" s="145"/>
       <c r="M7" s="32"/>
       <c r="N7" s="117">
         <v>7</v>
@@ -25497,10 +25504,10 @@
         <f t="shared" si="3"/>
         <v>165</v>
       </c>
-      <c r="D8" s="151" t="s">
+      <c r="D8" s="135" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="144"/>
+      <c r="E8" s="145"/>
       <c r="F8" s="81"/>
       <c r="G8" s="112">
         <f>Manager!T7</f>
@@ -25522,7 +25529,7 @@
         <f>SUM(K3/5)</f>
         <v>0</v>
       </c>
-      <c r="L8" s="144"/>
+      <c r="L8" s="145"/>
       <c r="M8" s="32"/>
       <c r="N8" s="117">
         <v>7</v>
@@ -25563,10 +25570,10 @@
         <f t="shared" si="4"/>
         <v>165</v>
       </c>
-      <c r="D9" s="151" t="s">
+      <c r="D9" s="135" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="144"/>
+      <c r="E9" s="145"/>
       <c r="F9" s="81"/>
       <c r="G9" s="112">
         <f>Manager!T8</f>
@@ -25588,7 +25595,7 @@
         <f>SUM(K3/5)</f>
         <v>0</v>
       </c>
-      <c r="L9" s="144"/>
+      <c r="L9" s="145"/>
       <c r="M9" s="32"/>
       <c r="N9" s="117">
         <v>7</v>
@@ -25622,7 +25629,7 @@
       <c r="B10" s="120"/>
       <c r="C10" s="120"/>
       <c r="D10" s="121"/>
-      <c r="E10" s="144"/>
+      <c r="E10" s="145"/>
       <c r="F10" s="81"/>
       <c r="G10" s="122">
         <f>SUM(G5:G9)</f>
@@ -25632,7 +25639,7 @@
       <c r="I10" s="123"/>
       <c r="J10" s="123"/>
       <c r="K10" s="29"/>
-      <c r="L10" s="144"/>
+      <c r="L10" s="145"/>
       <c r="M10" s="32"/>
       <c r="N10" s="124"/>
       <c r="O10" s="125"/>
@@ -43504,10 +43511,10 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" customHeight="1">
-      <c r="G2" s="149" t="s">
+      <c r="G2" s="150" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="144"/>
+      <c r="H2" s="145"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" customHeight="1">
       <c r="B3" s="130" t="s">

</xml_diff>